<commit_message>
Rerun the example data
</commit_message>
<xml_diff>
--- a/example-output/EXAMPLE_HOSPITAL/transmission-analysis_SNPcutoff20_Days45/CoreSNPclusters_ST152_SNPcutoff20_Days45.xlsx
+++ b/example-output/EXAMPLE_HOSPITAL/transmission-analysis_SNPcutoff20_Days45/CoreSNPclusters_ST152_SNPcutoff20_Days45.xlsx
@@ -65,7 +65,7 @@
     <t xml:space="preserve">2019.46</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
+    <t xml:space="preserve">3</t>
   </si>
   <si>
     <t xml:space="preserve">UNKNOWN</t>
@@ -150,9 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -189,7 +187,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>